<commit_message>
Minor Updates to icons and no feed simulation
</commit_message>
<xml_diff>
--- a/documents/sprint1/sprint-planning/elppa-sprint-backlog.xlsx
+++ b/documents/sprint1/sprint-planning/elppa-sprint-backlog.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="58">
   <si>
     <t>Comments</t>
   </si>
@@ -113,12 +113,6 @@
     <t>Day 10</t>
   </si>
   <si>
-    <t>Day 11</t>
-  </si>
-  <si>
-    <t>Day 12</t>
-  </si>
-  <si>
     <t>Effort Remaining</t>
   </si>
   <si>
@@ -173,15 +167,6 @@
     <t>Refactor Sprint 0 code where necessary</t>
   </si>
   <si>
-    <t>Research individual task</t>
-  </si>
-  <si>
-    <t>Refactor</t>
-  </si>
-  <si>
-    <t>Refactor`</t>
-  </si>
-  <si>
     <t>Sprint 1 Planning Meeting</t>
   </si>
   <si>
@@ -192,6 +177,24 @@
   </si>
   <si>
     <t>In Progress</t>
+  </si>
+  <si>
+    <t>Perform Metrics</t>
+  </si>
+  <si>
+    <t>Docment metrics</t>
+  </si>
+  <si>
+    <t>Perform metrics</t>
+  </si>
+  <si>
+    <t>Document Metrics</t>
+  </si>
+  <si>
+    <t>Refactor (Pair Programming)</t>
+  </si>
+  <si>
+    <t>Decide code metrics for use this sprint</t>
   </si>
 </sst>
 </file>
@@ -624,6 +627,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -637,7 +641,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint Backlog'!$E$35</c:f>
+              <c:f>'Sprint Backlog'!$E$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -657,9 +661,9 @@
           </c:trendline>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint Backlog'!$F$5:$R$5</c:f>
+              <c:f>'Sprint Backlog'!$F$5:$P$5</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Day 0</c:v>
                 </c:pt>
@@ -693,50 +697,44 @@
                 <c:pt idx="10">
                   <c:v>Day 10</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>Day 11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Day 12</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint Backlog'!$F$35:$O$35</c:f>
+              <c:f>'Sprint Backlog'!$F$33:$O$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -753,11 +751,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="84495744"/>
-        <c:axId val="84534400"/>
+        <c:axId val="82529664"/>
+        <c:axId val="83956864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84495744"/>
+        <c:axId val="82529664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -766,7 +764,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84534400"/>
+        <c:crossAx val="83956864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -774,7 +772,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84534400"/>
+        <c:axId val="83956864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -785,13 +783,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84495744"/>
+        <c:crossAx val="82529664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1166,10 +1165,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:R43"/>
+  <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1182,18 +1181,18 @@
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:18" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:16" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" s="41" t="s">
         <v>11</v>
@@ -1202,13 +1201,13 @@
         <v>12</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E4" s="41" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="39" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G4" s="40"/>
       <c r="H4" s="40"/>
@@ -1220,10 +1219,8 @@
       <c r="N4" s="40"/>
       <c r="O4" s="40"/>
       <c r="P4" s="40"/>
-      <c r="Q4" s="40"/>
-      <c r="R4" s="40"/>
-    </row>
-    <row r="5" spans="1:18" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
       <c r="B5" s="37"/>
       <c r="C5" s="37"/>
@@ -1262,14 +1259,8 @@
       <c r="P5" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="R5" s="17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:16" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="38"/>
       <c r="B6" s="38"/>
       <c r="C6" s="38"/>
@@ -1319,16 +1310,8 @@
         <f>WORKDAY('Configuration Details'!$B$1,INT(RIGHT(P5,2)))</f>
         <v>41227</v>
       </c>
-      <c r="Q6" s="22">
-        <f>WORKDAY('Configuration Details'!$B$1,INT(RIGHT(Q5,2)))</f>
-        <v>41228</v>
-      </c>
-      <c r="R6" s="22">
-        <f>WORKDAY('Configuration Details'!$B$1,INT(RIGHT(R5,2)))</f>
-        <v>41229</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -1345,7 +1328,7 @@
       <c r="N7" s="10"/>
       <c r="O7" s="9"/>
     </row>
-    <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>10</v>
       </c>
@@ -1394,21 +1377,13 @@
         <v>Day 9</v>
       </c>
       <c r="P8" s="2" t="str">
-        <f t="shared" ref="P8:R8" si="1">P5</f>
+        <f t="shared" ref="P8" si="1">P5</f>
         <v>Day 10</v>
       </c>
-      <c r="Q8" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>Day 11</v>
-      </c>
-      <c r="R8" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>Day 12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B9" s="19">
         <v>1</v>
@@ -1421,7 +1396,7 @@
       </c>
       <c r="E9" s="35"/>
       <c r="F9" s="19">
-        <f t="shared" ref="F9:R17" si="2">$B9</f>
+        <f t="shared" ref="F9:P16" si="2">$B9</f>
         <v>1</v>
       </c>
       <c r="G9" s="19">
@@ -1454,16 +1429,10 @@
       <c r="P9" s="19">
         <v>0</v>
       </c>
-      <c r="Q9" s="19">
-        <v>0</v>
-      </c>
-      <c r="R9" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B10" s="19">
         <v>1</v>
@@ -1475,7 +1444,7 @@
         <v>28</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F10" s="19">
         <f t="shared" si="2"/>
@@ -1511,16 +1480,10 @@
       <c r="P10" s="19">
         <v>0</v>
       </c>
-      <c r="Q10" s="19">
-        <v>0</v>
-      </c>
-      <c r="R10" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B11" s="19">
         <v>1</v>
@@ -1532,7 +1495,7 @@
         <v>28</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F11" s="19">
         <f t="shared" si="2"/>
@@ -1543,53 +1506,36 @@
         <v>1</v>
       </c>
       <c r="H11" s="19">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I11" s="19">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" s="19">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11" s="19">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11" s="19">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11" s="19">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11" s="19">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O11" s="19">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P11" s="19">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q11" s="19">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="R11" s="19">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B12" s="19">
         <v>2</v>
@@ -1638,16 +1584,10 @@
       <c r="P12" s="19">
         <v>0</v>
       </c>
-      <c r="Q12" s="19">
-        <v>0</v>
-      </c>
-      <c r="R12" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B13" s="19">
         <v>5</v>
@@ -1656,7 +1596,7 @@
         <v>27</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E13" s="35"/>
       <c r="F13" s="19">
@@ -1676,117 +1616,87 @@
         <v>5</v>
       </c>
       <c r="J13" s="19">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K13" s="19">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L13" s="19">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M13" s="19">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N13" s="19">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O13" s="19">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="P13" s="19">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="Q13" s="19">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="R13" s="19">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B14" s="19">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="E14" s="28"/>
       <c r="F14" s="19">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G14" s="19">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H14" s="19">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I14" s="19">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J14" s="19">
-        <f t="shared" si="2"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K14" s="19">
-        <f t="shared" si="2"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="L14" s="19">
-        <f t="shared" si="2"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M14" s="19">
-        <f t="shared" si="2"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="N14" s="19">
-        <f t="shared" si="2"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="O14" s="19">
-        <f t="shared" si="2"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P14" s="19">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="Q14" s="19">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="R14" s="19">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28"/>
       <c r="B15" s="19"/>
       <c r="C15" s="18" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E15" s="28"/>
       <c r="F15" s="19">
@@ -1833,23 +1743,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q15" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R15" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="28"/>
       <c r="B16" s="19"/>
       <c r="C16" s="18" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E16" s="28"/>
       <c r="F16" s="19">
@@ -1896,1146 +1798,929 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q16" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R16" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="28"/>
-      <c r="F17" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H17" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K17" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L17" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M17" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N17" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O17" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P17" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q17" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R17" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="31"/>
-      <c r="O18" s="31"/>
-    </row>
-    <row r="19" spans="1:18" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="2" t="str">
-        <f t="shared" ref="F19:P19" si="3">F5</f>
+    </row>
+    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31"/>
+    </row>
+    <row r="18" spans="1:16" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="2" t="str">
+        <f t="shared" ref="F18:P18" si="3">F5</f>
         <v>Day 0</v>
       </c>
-      <c r="G19" s="2" t="str">
+      <c r="G18" s="2" t="str">
         <f t="shared" si="3"/>
         <v>Day 1</v>
       </c>
-      <c r="H19" s="2" t="str">
+      <c r="H18" s="2" t="str">
         <f t="shared" si="3"/>
         <v>Day 2</v>
       </c>
-      <c r="I19" s="2" t="str">
+      <c r="I18" s="2" t="str">
         <f t="shared" si="3"/>
         <v>Day 3</v>
       </c>
-      <c r="J19" s="2" t="str">
+      <c r="J18" s="2" t="str">
         <f t="shared" si="3"/>
         <v>Day 4</v>
       </c>
-      <c r="K19" s="2" t="str">
+      <c r="K18" s="2" t="str">
         <f t="shared" si="3"/>
         <v>Day 5</v>
       </c>
-      <c r="L19" s="2" t="str">
+      <c r="L18" s="2" t="str">
         <f t="shared" si="3"/>
         <v>Day 6</v>
       </c>
-      <c r="M19" s="2" t="str">
+      <c r="M18" s="2" t="str">
         <f t="shared" si="3"/>
         <v>Day 7</v>
       </c>
-      <c r="N19" s="2" t="str">
+      <c r="N18" s="2" t="str">
         <f t="shared" si="3"/>
         <v>Day 8</v>
       </c>
-      <c r="O19" s="2" t="str">
+      <c r="O18" s="2" t="str">
         <f t="shared" si="3"/>
         <v>Day 9</v>
       </c>
-      <c r="P19" s="2" t="str">
+      <c r="P18" s="2" t="str">
         <f t="shared" si="3"/>
         <v>Day 10</v>
       </c>
-      <c r="Q19" s="2" t="str">
-        <f t="shared" ref="Q19:R19" si="4">Q5</f>
-        <v>Day 11</v>
-      </c>
-      <c r="R19" s="2" t="str">
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="4">
+        <v>5</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3">
+        <f>$B19</f>
+        <v>5</v>
+      </c>
+      <c r="G19" s="3">
+        <f t="shared" ref="G19:J19" si="4">$B19</f>
+        <v>5</v>
+      </c>
+      <c r="H19" s="3">
         <f t="shared" si="4"/>
-        <v>Day 12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="30" t="s">
-        <v>47</v>
+        <v>5</v>
+      </c>
+      <c r="I19" s="3">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="J19" s="3">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="K19" s="3">
+        <v>0</v>
+      </c>
+      <c r="L19" s="3">
+        <v>0</v>
+      </c>
+      <c r="M19" s="3">
+        <v>0</v>
+      </c>
+      <c r="N19" s="3">
+        <v>0</v>
+      </c>
+      <c r="O19" s="3">
+        <v>0</v>
+      </c>
+      <c r="P19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="B20" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3">
-        <f>$B20</f>
-        <v>5</v>
+        <f t="shared" ref="F20:P24" si="5">$B20</f>
+        <v>2</v>
       </c>
       <c r="G20" s="3">
-        <f t="shared" ref="G20:R20" si="5">$B20</f>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="H20" s="3">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I20" s="3">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J20" s="3">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K20" s="3">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L20" s="3">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M20" s="3">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N20" s="3">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O20" s="3">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="P20" s="3">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="Q20" s="3">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="R20" s="3">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>48</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="s">
+        <v>56</v>
       </c>
       <c r="B21" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3">
-        <f t="shared" ref="F21:R25" si="6">$B21</f>
-        <v>2</v>
+        <f t="shared" si="5"/>
+        <v>5</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
+        <f t="shared" si="5"/>
+        <v>5</v>
       </c>
       <c r="H21" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
+        <f t="shared" si="5"/>
+        <v>5</v>
       </c>
       <c r="I21" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
+        <f t="shared" si="5"/>
+        <v>5</v>
       </c>
       <c r="J21" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
+        <f t="shared" si="5"/>
+        <v>5</v>
       </c>
       <c r="K21" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
+        <f t="shared" si="5"/>
+        <v>5</v>
       </c>
       <c r="L21" s="3">
-        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="M21" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N21" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O21" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P21" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="Q21" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="R21" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="29" t="s">
-        <v>51</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="B22" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3">
-        <f t="shared" si="6"/>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="G22" s="3">
-        <f t="shared" si="6"/>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="H22" s="3">
-        <f t="shared" si="6"/>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="I22" s="3">
-        <f t="shared" si="6"/>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="J22" s="3">
-        <f t="shared" si="6"/>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="K22" s="3">
-        <f t="shared" si="6"/>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="L22" s="3">
-        <f t="shared" si="6"/>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="M22" s="3">
-        <f t="shared" si="6"/>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="N22" s="3">
-        <f t="shared" si="6"/>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="O22" s="3">
-        <f t="shared" si="6"/>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="P22" s="3">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="Q22" s="3">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="R22" s="3">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="4">
+        <v>2</v>
+      </c>
       <c r="C23" s="18" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="G23" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="H23" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="I23" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="J23" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="K23" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="L23" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="M23" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="N23" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="O23" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="P23" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q23" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="R23" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="29"/>
       <c r="B24" s="4"/>
       <c r="C24" s="18" t="s">
         <v>17</v>
       </c>
       <c r="D24" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="6"/>
+      <c r="F24" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L24" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N24" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O24" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P24" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="13"/>
+    </row>
+    <row r="26" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="2" t="str">
+        <f t="shared" ref="F26:P26" si="6">F5</f>
+        <v>Day 0</v>
+      </c>
+      <c r="G26" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>Day 1</v>
+      </c>
+      <c r="H26" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>Day 2</v>
+      </c>
+      <c r="I26" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>Day 3</v>
+      </c>
+      <c r="J26" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>Day 4</v>
+      </c>
+      <c r="K26" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>Day 5</v>
+      </c>
+      <c r="L26" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>Day 6</v>
+      </c>
+      <c r="M26" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>Day 7</v>
+      </c>
+      <c r="N26" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>Day 8</v>
+      </c>
+      <c r="O26" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>Day 9</v>
+      </c>
+      <c r="P26" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>Day 10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="4">
+        <v>5</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G24" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="H24" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I24" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J24" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K24" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L24" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M24" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="N24" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="O24" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P24" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q24" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="R24" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="29"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="18" t="s">
+      <c r="E27" s="4"/>
+      <c r="F27" s="4">
+        <f>$B27</f>
+        <v>5</v>
+      </c>
+      <c r="G27" s="4">
+        <f t="shared" ref="G27:M27" si="7">$B27</f>
+        <v>5</v>
+      </c>
+      <c r="H27" s="4">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="I27" s="4">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="J27" s="4">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="K27" s="4">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="L27" s="4">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="M27" s="4">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="N27" s="4">
+        <v>3</v>
+      </c>
+      <c r="O27" s="4">
+        <v>0</v>
+      </c>
+      <c r="P27" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="4">
+        <v>2</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="4">
+        <f t="shared" ref="F28:P32" si="8">$B28</f>
+        <v>2</v>
+      </c>
+      <c r="G28" s="4">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="H28" s="4">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="I28" s="4">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="J28" s="4">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="K28" s="4">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="L28" s="4">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="M28" s="4">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="N28" s="4">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="O28" s="4">
+        <v>0</v>
+      </c>
+      <c r="P28" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="4">
+        <v>5</v>
+      </c>
+      <c r="C29" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="6"/>
-      <c r="F25" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="H25" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J25" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K25" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L25" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M25" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="N25" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="O25" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P25" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q25" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="R25" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="13"/>
-    </row>
-    <row r="27" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="2" t="str">
-        <f t="shared" ref="F27:P27" si="7">F5</f>
-        <v>Day 0</v>
-      </c>
-      <c r="G27" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>Day 1</v>
-      </c>
-      <c r="H27" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>Day 2</v>
-      </c>
-      <c r="I27" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>Day 3</v>
-      </c>
-      <c r="J27" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>Day 4</v>
-      </c>
-      <c r="K27" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>Day 5</v>
-      </c>
-      <c r="L27" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>Day 6</v>
-      </c>
-      <c r="M27" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>Day 7</v>
-      </c>
-      <c r="N27" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>Day 8</v>
-      </c>
-      <c r="O27" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>Day 9</v>
-      </c>
-      <c r="P27" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>Day 10</v>
-      </c>
-      <c r="Q27" s="2" t="str">
-        <f t="shared" ref="Q27:R27" si="8">Q5</f>
-        <v>Day 11</v>
-      </c>
-      <c r="R27" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>Day 12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B28" s="4">
-        <v>5</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4">
-        <f>$B28</f>
-        <v>5</v>
-      </c>
-      <c r="G28" s="4">
-        <f t="shared" ref="G28:R28" si="9">$B28</f>
-        <v>5</v>
-      </c>
-      <c r="H28" s="4">
-        <f t="shared" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="I28" s="4">
-        <f t="shared" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="J28" s="4">
-        <f t="shared" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="K28" s="4">
-        <f t="shared" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="L28" s="4">
-        <f t="shared" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="M28" s="4">
-        <f t="shared" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="N28" s="4">
-        <f t="shared" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="O28" s="4">
-        <f t="shared" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="P28" s="4">
-        <f t="shared" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="Q28" s="4">
-        <f t="shared" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="R28" s="4">
-        <f t="shared" si="9"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="4">
-        <v>2</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>27</v>
-      </c>
       <c r="D29" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="4">
-        <f t="shared" ref="F29:R33" si="10">$B29</f>
-        <v>2</v>
+        <f t="shared" si="8"/>
+        <v>5</v>
       </c>
       <c r="G29" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
+        <f t="shared" si="8"/>
+        <v>5</v>
       </c>
       <c r="H29" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
+        <f t="shared" si="8"/>
+        <v>5</v>
       </c>
       <c r="I29" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
+        <f t="shared" si="8"/>
+        <v>5</v>
       </c>
       <c r="J29" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
+        <f t="shared" si="8"/>
+        <v>5</v>
       </c>
       <c r="K29" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
+        <f t="shared" si="8"/>
+        <v>5</v>
       </c>
       <c r="L29" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
+        <f t="shared" si="8"/>
+        <v>5</v>
       </c>
       <c r="M29" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
+        <f t="shared" si="8"/>
+        <v>5</v>
       </c>
       <c r="N29" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
+        <f t="shared" si="8"/>
+        <v>5</v>
       </c>
       <c r="O29" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P29" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-      <c r="Q29" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-      <c r="R29" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="29" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B30" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>54</v>
+        <v>18</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="4">
-        <f t="shared" si="10"/>
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>2</v>
       </c>
       <c r="G30" s="4">
-        <f t="shared" si="10"/>
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>2</v>
       </c>
       <c r="H30" s="4">
-        <f t="shared" si="10"/>
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>2</v>
       </c>
       <c r="I30" s="4">
-        <f t="shared" si="10"/>
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>2</v>
       </c>
       <c r="J30" s="4">
-        <f t="shared" si="10"/>
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>2</v>
       </c>
       <c r="K30" s="4">
-        <f t="shared" si="10"/>
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>2</v>
       </c>
       <c r="L30" s="4">
-        <f t="shared" si="10"/>
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>2</v>
       </c>
       <c r="M30" s="4">
-        <f t="shared" si="10"/>
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>2</v>
       </c>
       <c r="N30" s="4">
-        <f t="shared" si="10"/>
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>2</v>
       </c>
       <c r="O30" s="4">
-        <f t="shared" si="10"/>
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>2</v>
       </c>
       <c r="P30" s="4">
-        <f t="shared" si="10"/>
-        <v>5</v>
-      </c>
-      <c r="Q30" s="4">
-        <f t="shared" si="10"/>
-        <v>5</v>
-      </c>
-      <c r="R30" s="4">
-        <f t="shared" si="10"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="4">
+        <v>2</v>
+      </c>
       <c r="C31" s="18" t="s">
         <v>18</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>2</v>
       </c>
       <c r="G31" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>2</v>
       </c>
       <c r="H31" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>2</v>
       </c>
       <c r="I31" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>2</v>
       </c>
       <c r="J31" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>2</v>
       </c>
       <c r="K31" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>2</v>
       </c>
       <c r="L31" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>2</v>
       </c>
       <c r="M31" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>2</v>
       </c>
       <c r="N31" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>2</v>
       </c>
       <c r="O31" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>2</v>
       </c>
       <c r="P31" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="Q31" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="R31" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="29"/>
       <c r="B32" s="4"/>
       <c r="C32" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E32" s="3"/>
+      <c r="D32" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" s="6"/>
       <c r="F32" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G32" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H32" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I32" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J32" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K32" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L32" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M32" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="N32" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O32" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P32" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="Q32" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="R32" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="29"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="18" t="s">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="E33" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" s="4">
+        <f>SUM(F9:F16,F19:F24,F27:F32)</f>
+        <v>43</v>
+      </c>
+      <c r="G33" s="4">
+        <f t="shared" ref="G33:P33" si="9">SUM(G9:G16,G19:G24,G27:G32)</f>
+        <v>41</v>
+      </c>
+      <c r="H33" s="4">
+        <f t="shared" si="9"/>
+        <v>42</v>
+      </c>
+      <c r="I33" s="4">
+        <f t="shared" si="9"/>
+        <v>40</v>
+      </c>
+      <c r="J33" s="4">
+        <f t="shared" si="9"/>
+        <v>36</v>
+      </c>
+      <c r="K33" s="4">
+        <f t="shared" si="9"/>
+        <v>30</v>
+      </c>
+      <c r="L33" s="4">
+        <f t="shared" si="9"/>
+        <v>23</v>
+      </c>
+      <c r="M33" s="4">
+        <f t="shared" si="9"/>
+        <v>22</v>
+      </c>
+      <c r="N33" s="4">
+        <f t="shared" si="9"/>
         <v>18</v>
       </c>
-      <c r="D33" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E33" s="6"/>
-      <c r="F33" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="G33" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="H33" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I33" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="J33" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="K33" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="L33" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="M33" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="N33" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
       <c r="O33" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>8</v>
       </c>
       <c r="P33" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="Q33" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="R33" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
-      <c r="M34" s="5"/>
-      <c r="N34" s="5"/>
-      <c r="O34" s="13"/>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E35" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="F35" s="4">
-        <f t="shared" ref="F35:R35" si="11">$B35</f>
-        <v>0</v>
-      </c>
-      <c r="G35" s="4">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="H35" s="4">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="I35" s="4">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J35" s="4">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="K35" s="4">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="L35" s="4">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="M35" s="4">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="N35" s="4">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="O35" s="4">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="P35" s="4">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="Q35" s="4">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="R35" s="4">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="25" t="s">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="27">
-        <f>SUM(B9:B17,B20:B25,B28:B33)</f>
-        <v>44</v>
-      </c>
-      <c r="C38" s="26" t="s">
+      <c r="B36" s="27">
+        <f>SUM(B9:B16,B19:B24,B27:B32)</f>
+        <v>43</v>
+      </c>
+      <c r="C36" s="26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="20"/>
-    </row>
-    <row r="40" spans="1:18" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="23" t="s">
+    <row r="37" spans="1:16" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="20"/>
+    </row>
+    <row r="38" spans="1:16" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="3"/>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="3">
+        <f>COUNTIF($D$9:$D$32,"Not Started")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" s="3">
+        <f>COUNTIF($D$9:$D$32,"In Progress")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B41" s="3">
-        <f>COUNTIF($D$9:$D$34,"Not Started")</f>
+        <f>COUNTIF($D$9:$D$32,"Complete")</f>
         <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B42" s="3">
-        <f>COUNTIF($D$9:$D$34,"In Progress")</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B43" s="3">
-        <f>COUNTIF($D$9:$D$33,"Complete")</f>
-        <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A4:A6"/>
-    <mergeCell ref="F4:R4"/>
+    <mergeCell ref="F4:P4"/>
     <mergeCell ref="E4:E6"/>
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="D4:D6"/>
   </mergeCells>
-  <conditionalFormatting sqref="C26:C27 D9:D17 D20:D25 D28:D33">
+  <conditionalFormatting sqref="C25:C26 D19:D24 D27:D32 D9:D16">
     <cfRule type="containsText" dxfId="2" priority="14" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",C9)))</formula>
     </cfRule>
@@ -3043,13 +2728,13 @@
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D9:D17 D20:D25 C27:D380">
+  <conditionalFormatting sqref="D19:D24 D9:D16 C26:D378">
     <cfRule type="containsText" dxfId="0" priority="13" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Choice" error="Plese select an option from the drop-down list." sqref="D9:D17 C26:C27 D20:D25 D28:D33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Choice" error="Plese select an option from the drop-down list." sqref="C25:C26 D19:D24 D27:D32 D9:D16">
       <formula1>"Not Started, In Progress, Complete"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3062,7 +2747,7 @@
           <x14:formula1>
             <xm:f>'Configuration Details'!$A$4:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C20:C25 C9:C17 C28:C33</xm:sqref>
+          <xm:sqref>C19:C24 C27:C32 C9:C16</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3126,7 +2811,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3134,7 +2819,7 @@
         <v>27</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3142,7 +2827,7 @@
         <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3150,7 +2835,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>